<commit_message>
Ajout liens man synthèse UNIX
</commit_message>
<xml_diff>
--- a/Synthèse Anglais/Vocabulaire_Anglais.xlsx
+++ b/Synthèse Anglais/Vocabulaire_Anglais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulaire" sheetId="1" r:id="rId1"/>
@@ -3850,7 +3850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C405"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A391" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7160,15 +7160,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>